<commit_message>
[WIP] Fix adjust to contents
</commit_message>
<xml_diff>
--- a/ClosedXML.Tests/Resource/Examples/Misc/AdjustToContents.xlsx
+++ b/ClosedXML.Tests/Resource/Examples/Misc/AdjustToContents.xlsx
@@ -3400,16 +3400,16 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="30.790625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="28.190625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="30.79" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="28.19" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
-    <x:row r="1" spans="1:2" customFormat="1" ht="41.5039" customHeight="1">
+    <x:row r="1" spans="1:2" customFormat="1" ht="41.5" customHeight="1">
       <x:c r="A1" s="1" t="s">
         <x:v>0</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:2" customFormat="1" ht="27.669267" customHeight="1">
+    <x:row r="2" spans="1:2" customFormat="1" ht="27.67" customHeight="1">
       <x:c r="A2" s="2" t="s">
         <x:v>1</x:v>
       </x:c>
@@ -3462,25 +3462,25 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="2.930625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="16.150625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="17.315676" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="18.195145" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="17.902475" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="17.495861" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="16.978396" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="16.354019" style="0" customWidth="1"/>
-    <x:col min="9" max="9" width="15.627482" style="0" customWidth="1"/>
-    <x:col min="10" max="10" width="14.804314" style="0" customWidth="1"/>
-    <x:col min="11" max="11" width="13.89078" style="0" customWidth="1"/>
-    <x:col min="12" max="12" width="12.893833" style="0" customWidth="1"/>
-    <x:col min="13" max="13" width="11.82106" style="0" customWidth="1"/>
-    <x:col min="14" max="14" width="10.680625" style="0" customWidth="1"/>
-    <x:col min="15" max="15" width="9.481208" style="0" customWidth="1"/>
-    <x:col min="16" max="16" width="8.231937" style="0" customWidth="1"/>
-    <x:col min="17" max="17" width="6.94232" style="0" customWidth="1"/>
-    <x:col min="18" max="18" width="5.622172" style="0" customWidth="1"/>
-    <x:col min="19" max="19" width="4.281539" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="2.93" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="16.15" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="17.31" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="18.19" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="17.9" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="17.49" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="16.97" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="16.35" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="15.62" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="14.8" style="0" customWidth="1"/>
+    <x:col min="11" max="11" width="13.89" style="0" customWidth="1"/>
+    <x:col min="12" max="12" width="12.89" style="0" customWidth="1"/>
+    <x:col min="13" max="13" width="11.82" style="0" customWidth="1"/>
+    <x:col min="14" max="14" width="10.68" style="0" customWidth="1"/>
+    <x:col min="15" max="15" width="9.48" style="0" customWidth="1"/>
+    <x:col min="16" max="16" width="8.23" style="0" customWidth="1"/>
+    <x:col min="17" max="17" width="6.94" style="0" customWidth="1"/>
+    <x:col min="18" max="18" width="5.62" style="0" customWidth="1"/>
+    <x:col min="19" max="19" width="4.28" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:19">
@@ -3562,25 +3562,25 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="2.930625" style="0" customWidth="1"/>
-    <x:col min="2" max="2" width="51.020625" style="0" customWidth="1"/>
-    <x:col min="3" max="3" width="61.832986" style="0" customWidth="1"/>
-    <x:col min="4" max="4" width="61.271495" style="0" customWidth="1"/>
-    <x:col min="5" max="5" width="60.340427" style="0" customWidth="1"/>
-    <x:col min="6" max="6" width="59.046868" style="0" customWidth="1"/>
-    <x:col min="7" max="7" width="57.400662" style="0" customWidth="1"/>
-    <x:col min="8" max="8" width="55.414338" style="0" customWidth="1"/>
-    <x:col min="9" max="9" width="53.103012" style="0" customWidth="1"/>
-    <x:col min="10" max="10" width="50.484276" style="0" customWidth="1"/>
-    <x:col min="11" max="11" width="47.57806" style="0" customWidth="1"/>
-    <x:col min="12" max="12" width="44.406482" style="0" customWidth="1"/>
-    <x:col min="13" max="13" width="40.993679" style="0" customWidth="1"/>
-    <x:col min="14" max="14" width="37.365625" style="0" customWidth="1"/>
-    <x:col min="15" max="15" width="33.549931" style="0" customWidth="1"/>
-    <x:col min="16" max="16" width="29.575638" style="0" customWidth="1"/>
-    <x:col min="17" max="17" width="25.472992" style="0" customWidth="1"/>
-    <x:col min="18" max="18" width="21.273217" style="0" customWidth="1"/>
-    <x:col min="19" max="19" width="17.008275" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="2.93" style="0" customWidth="1"/>
+    <x:col min="2" max="2" width="51.02" style="0" customWidth="1"/>
+    <x:col min="3" max="3" width="61.84" style="0" customWidth="1"/>
+    <x:col min="4" max="4" width="61.28" style="0" customWidth="1"/>
+    <x:col min="5" max="5" width="60.35" style="0" customWidth="1"/>
+    <x:col min="6" max="6" width="59.05" style="0" customWidth="1"/>
+    <x:col min="7" max="7" width="57.41" style="0" customWidth="1"/>
+    <x:col min="8" max="8" width="55.42" style="0" customWidth="1"/>
+    <x:col min="9" max="9" width="53.11" style="0" customWidth="1"/>
+    <x:col min="10" max="10" width="50.49" style="0" customWidth="1"/>
+    <x:col min="11" max="11" width="47.58" style="0" customWidth="1"/>
+    <x:col min="12" max="12" width="44.41" style="0" customWidth="1"/>
+    <x:col min="13" max="13" width="41" style="0" customWidth="1"/>
+    <x:col min="14" max="14" width="37.37" style="0" customWidth="1"/>
+    <x:col min="15" max="15" width="33.56" style="0" customWidth="1"/>
+    <x:col min="16" max="16" width="29.58" style="0" customWidth="1"/>
+    <x:col min="17" max="17" width="25.48" style="0" customWidth="1"/>
+    <x:col min="18" max="18" width="21.28" style="0" customWidth="1"/>
+    <x:col min="19" max="19" width="17.02" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>
     <x:row r="1" spans="1:19">
@@ -3662,97 +3662,97 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:1" customFormat="1" ht="304.361925" customHeight="1">
+    <x:row r="1" spans="1:1" customFormat="1" ht="304.36" customHeight="1">
       <x:c r="A1" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:1" customFormat="1" ht="15.218096" customHeight="1">
+    <x:row r="2" spans="1:1" customFormat="1" ht="15.22" customHeight="1">
       <x:c r="A2" s="0" t="s">
         <x:v>7</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:1" customFormat="1" ht="7.609048" customHeight="1">
+    <x:row r="3" spans="1:1" customFormat="1" ht="7.61" customHeight="1">
       <x:c r="A3" s="4" t="s">
         <x:v>8</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:1" customFormat="1" ht="16.063546" customHeight="1">
+    <x:row r="4" spans="1:1" customFormat="1" ht="16.06" customHeight="1">
       <x:c r="A4" s="5" t="s">
         <x:v>9</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:1" customFormat="1" ht="24.095319" customHeight="1">
+    <x:row r="5" spans="1:1" customFormat="1" ht="24.1" customHeight="1">
       <x:c r="A5" s="6" t="s">
         <x:v>10</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:1" customFormat="1" ht="32.127092" customHeight="1">
+    <x:row r="6" spans="1:1" customFormat="1" ht="32.13" customHeight="1">
       <x:c r="A6" s="7" t="s">
         <x:v>11</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:1" customFormat="1" ht="40.158865" customHeight="1">
+    <x:row r="7" spans="1:1" customFormat="1" ht="40.16" customHeight="1">
       <x:c r="A7" s="8" t="s">
         <x:v>12</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:1" customFormat="1" ht="48.190638" customHeight="1">
+    <x:row r="8" spans="1:1" customFormat="1" ht="48.19" customHeight="1">
       <x:c r="A8" s="9" t="s">
         <x:v>13</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:1" customFormat="1" ht="56.222411" customHeight="1">
+    <x:row r="9" spans="1:1" customFormat="1" ht="56.22" customHeight="1">
       <x:c r="A9" s="10" t="s">
         <x:v>14</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:1" customFormat="1" ht="64.254184" customHeight="1">
+    <x:row r="10" spans="1:1" customFormat="1" ht="64.25" customHeight="1">
       <x:c r="A10" s="11" t="s">
         <x:v>15</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:1" customFormat="1" ht="72.285957" customHeight="1">
+    <x:row r="11" spans="1:1" customFormat="1" ht="72.29" customHeight="1">
       <x:c r="A11" s="12" t="s">
         <x:v>16</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:1" customFormat="1" ht="80.31773" customHeight="1">
+    <x:row r="12" spans="1:1" customFormat="1" ht="80.32" customHeight="1">
       <x:c r="A12" s="13" t="s">
         <x:v>17</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:1" customFormat="1" ht="88.349503" customHeight="1">
+    <x:row r="13" spans="1:1" customFormat="1" ht="88.35" customHeight="1">
       <x:c r="A13" s="14" t="s">
         <x:v>18</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:1" customFormat="1" ht="96.381276" customHeight="1">
+    <x:row r="14" spans="1:1" customFormat="1" ht="96.38" customHeight="1">
       <x:c r="A14" s="15" t="s">
         <x:v>19</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:1" customFormat="1" ht="104.413049" customHeight="1">
+    <x:row r="15" spans="1:1" customFormat="1" ht="104.41" customHeight="1">
       <x:c r="A15" s="16" t="s">
         <x:v>20</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:1" customFormat="1" ht="112.444822" customHeight="1">
+    <x:row r="16" spans="1:1" customFormat="1" ht="112.44" customHeight="1">
       <x:c r="A16" s="17" t="s">
         <x:v>21</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:1" customFormat="1" ht="120.476595" customHeight="1">
+    <x:row r="17" spans="1:1" customFormat="1" ht="120.48" customHeight="1">
       <x:c r="A17" s="18" t="s">
         <x:v>22</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:1" customFormat="1" ht="128.508368" customHeight="1">
+    <x:row r="18" spans="1:1" customFormat="1" ht="128.51" customHeight="1">
       <x:c r="A18" s="19" t="s">
         <x:v>23</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:1" customFormat="1" ht="136.540141" customHeight="1">
+    <x:row r="19" spans="1:1" customFormat="1" ht="136.54" customHeight="1">
       <x:c r="A19" s="20" t="s">
         <x:v>24</x:v>
       </x:c>
@@ -3777,97 +3777,97 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:1" customFormat="1" ht="304.361925" customHeight="1">
+    <x:row r="1" spans="1:1" customFormat="1" ht="304.36" customHeight="1">
       <x:c r="A1" s="3" t="s">
         <x:v>6</x:v>
       </x:c>
     </x:row>
-    <x:row r="2" spans="1:1" customFormat="1" ht="83.0078" customHeight="1">
+    <x:row r="2" spans="1:1" customFormat="1" ht="83.01" customHeight="1">
       <x:c r="A2" s="0" t="s">
         <x:v>43</x:v>
       </x:c>
     </x:row>
-    <x:row r="3" spans="1:1" customFormat="1" ht="17.293292" customHeight="1">
+    <x:row r="3" spans="1:1" customFormat="1" ht="17.29" customHeight="1">
       <x:c r="A3" s="4" t="s">
         <x:v>44</x:v>
       </x:c>
     </x:row>
-    <x:row r="4" spans="1:1" customFormat="1" ht="34.586583" customHeight="1">
+    <x:row r="4" spans="1:1" customFormat="1" ht="34.59" customHeight="1">
       <x:c r="A4" s="5" t="s">
         <x:v>45</x:v>
       </x:c>
     </x:row>
-    <x:row r="5" spans="1:1" customFormat="1" ht="51.879875" customHeight="1">
+    <x:row r="5" spans="1:1" customFormat="1" ht="51.88" customHeight="1">
       <x:c r="A5" s="6" t="s">
         <x:v>46</x:v>
       </x:c>
     </x:row>
-    <x:row r="6" spans="1:1" customFormat="1" ht="69.173166" customHeight="1">
+    <x:row r="6" spans="1:1" customFormat="1" ht="69.17" customHeight="1">
       <x:c r="A6" s="7" t="s">
         <x:v>47</x:v>
       </x:c>
     </x:row>
-    <x:row r="7" spans="1:1" customFormat="1" ht="86.466458" customHeight="1">
+    <x:row r="7" spans="1:1" customFormat="1" ht="86.47" customHeight="1">
       <x:c r="A7" s="8" t="s">
         <x:v>48</x:v>
       </x:c>
     </x:row>
-    <x:row r="8" spans="1:1" customFormat="1" ht="103.759749" customHeight="1">
+    <x:row r="8" spans="1:1" customFormat="1" ht="103.76" customHeight="1">
       <x:c r="A8" s="9" t="s">
         <x:v>49</x:v>
       </x:c>
     </x:row>
-    <x:row r="9" spans="1:1" customFormat="1" ht="121.053041" customHeight="1">
+    <x:row r="9" spans="1:1" customFormat="1" ht="121.05" customHeight="1">
       <x:c r="A9" s="10" t="s">
         <x:v>50</x:v>
       </x:c>
     </x:row>
-    <x:row r="10" spans="1:1" customFormat="1" ht="138.346333" customHeight="1">
+    <x:row r="10" spans="1:1" customFormat="1" ht="138.35" customHeight="1">
       <x:c r="A10" s="11" t="s">
         <x:v>51</x:v>
       </x:c>
     </x:row>
-    <x:row r="11" spans="1:1" customFormat="1" ht="155.639624" customHeight="1">
+    <x:row r="11" spans="1:1" customFormat="1" ht="155.64" customHeight="1">
       <x:c r="A11" s="12" t="s">
         <x:v>52</x:v>
       </x:c>
     </x:row>
-    <x:row r="12" spans="1:1" customFormat="1" ht="172.932916" customHeight="1">
+    <x:row r="12" spans="1:1" customFormat="1" ht="172.93" customHeight="1">
       <x:c r="A12" s="13" t="s">
         <x:v>53</x:v>
       </x:c>
     </x:row>
-    <x:row r="13" spans="1:1" customFormat="1" ht="190.226207" customHeight="1">
+    <x:row r="13" spans="1:1" customFormat="1" ht="190.23" customHeight="1">
       <x:c r="A13" s="14" t="s">
         <x:v>54</x:v>
       </x:c>
     </x:row>
-    <x:row r="14" spans="1:1" customFormat="1" ht="207.519499" customHeight="1">
+    <x:row r="14" spans="1:1" customFormat="1" ht="207.52" customHeight="1">
       <x:c r="A14" s="15" t="s">
         <x:v>55</x:v>
       </x:c>
     </x:row>
-    <x:row r="15" spans="1:1" customFormat="1" ht="224.81279" customHeight="1">
+    <x:row r="15" spans="1:1" customFormat="1" ht="224.81" customHeight="1">
       <x:c r="A15" s="16" t="s">
         <x:v>56</x:v>
       </x:c>
     </x:row>
-    <x:row r="16" spans="1:1" customFormat="1" ht="242.106082" customHeight="1">
+    <x:row r="16" spans="1:1" customFormat="1" ht="242.11" customHeight="1">
       <x:c r="A16" s="17" t="s">
         <x:v>57</x:v>
       </x:c>
     </x:row>
-    <x:row r="17" spans="1:1" customFormat="1" ht="259.399374" customHeight="1">
+    <x:row r="17" spans="1:1" customFormat="1" ht="259.4" customHeight="1">
       <x:c r="A17" s="18" t="s">
         <x:v>58</x:v>
       </x:c>
     </x:row>
-    <x:row r="18" spans="1:1" customFormat="1" ht="276.692665" customHeight="1">
+    <x:row r="18" spans="1:1" customFormat="1" ht="276.69" customHeight="1">
       <x:c r="A18" s="19" t="s">
         <x:v>59</x:v>
       </x:c>
     </x:row>
-    <x:row r="19" spans="1:1" customFormat="1" ht="293.985957" customHeight="1">
+    <x:row r="19" spans="1:1" customFormat="1" ht="293.99" customHeight="1">
       <x:c r="A19" s="20" t="s">
         <x:v>60</x:v>
       </x:c>
@@ -3892,7 +3892,7 @@
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:cols>
-    <x:col min="1" max="1" width="11.920625" style="0" customWidth="1"/>
+    <x:col min="1" max="1" width="11.92" style="0" customWidth="1"/>
     <x:col min="2" max="2" width="255" style="0" customWidth="1"/>
   </x:cols>
   <x:sheetData>

</xml_diff>